<commit_message>
Finalized logic and display score
</commit_message>
<xml_diff>
--- a/public/images/excel-march-madness.xlsx
+++ b/public/images/excel-march-madness.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="25600" windowHeight="13880"/>
+    <workbookView xWindow="1600" yWindow="0" windowWidth="25600" windowHeight="13880"/>
   </bookViews>
   <sheets>
     <sheet name="madness" sheetId="1" r:id="rId1"/>
@@ -868,9 +868,82 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -900,6 +973,14 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -941,111 +1022,30 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="24" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1403,260 +1403,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="79.5" customHeight="1">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="107"/>
-      <c r="Y1" s="107"/>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="107"/>
-      <c r="AB1" s="107"/>
-      <c r="AC1" s="107"/>
-      <c r="AD1" s="107"/>
-      <c r="AE1" s="107"/>
-      <c r="AF1" s="107"/>
-      <c r="AG1" s="107"/>
-      <c r="AH1" s="107"/>
-      <c r="AI1" s="107"/>
-      <c r="AJ1" s="107"/>
-      <c r="AK1" s="107"/>
-      <c r="AL1" s="107"/>
-      <c r="AM1" s="107"/>
-      <c r="AN1" s="107"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
+      <c r="S1" s="131"/>
+      <c r="T1" s="131"/>
+      <c r="U1" s="131"/>
+      <c r="V1" s="131"/>
+      <c r="W1" s="131"/>
+      <c r="X1" s="131"/>
+      <c r="Y1" s="131"/>
+      <c r="Z1" s="131"/>
+      <c r="AA1" s="131"/>
+      <c r="AB1" s="131"/>
+      <c r="AC1" s="131"/>
+      <c r="AD1" s="131"/>
+      <c r="AE1" s="131"/>
+      <c r="AF1" s="131"/>
+      <c r="AG1" s="131"/>
+      <c r="AH1" s="131"/>
+      <c r="AI1" s="131"/>
+      <c r="AJ1" s="131"/>
+      <c r="AK1" s="131"/>
+      <c r="AL1" s="131"/>
+      <c r="AM1" s="131"/>
+      <c r="AN1" s="131"/>
     </row>
     <row r="2" spans="1:40" s="7" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="107"/>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="107"/>
-      <c r="AE2" s="107"/>
-      <c r="AF2" s="107"/>
-      <c r="AG2" s="107"/>
-      <c r="AH2" s="107"/>
-      <c r="AI2" s="107"/>
-      <c r="AJ2" s="107"/>
-      <c r="AK2" s="107"/>
-      <c r="AL2" s="107"/>
-      <c r="AM2" s="107"/>
-      <c r="AN2" s="107"/>
-    </row>
-    <row r="3" spans="1:40" s="125" customFormat="1" ht="22" customHeight="1">
-      <c r="A3" s="127"/>
-      <c r="B3" s="128" t="s">
+      <c r="A2" s="131"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="131"/>
+      <c r="Z2" s="131"/>
+      <c r="AA2" s="131"/>
+      <c r="AB2" s="131"/>
+      <c r="AC2" s="131"/>
+      <c r="AD2" s="131"/>
+      <c r="AE2" s="131"/>
+      <c r="AF2" s="131"/>
+      <c r="AG2" s="131"/>
+      <c r="AH2" s="131"/>
+      <c r="AI2" s="131"/>
+      <c r="AJ2" s="131"/>
+      <c r="AK2" s="131"/>
+      <c r="AL2" s="131"/>
+      <c r="AM2" s="131"/>
+      <c r="AN2" s="131"/>
+    </row>
+    <row r="3" spans="1:40" s="103" customFormat="1" ht="22" customHeight="1">
+      <c r="A3" s="105"/>
+      <c r="B3" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="128"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129" t="s">
+      <c r="C3" s="152"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129" t="s">
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129" t="s">
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="129" t="s">
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="130"/>
-      <c r="P3" s="130"/>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="128" t="s">
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
+      <c r="Q3" s="107"/>
+      <c r="R3" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="128"/>
-      <c r="T3" s="128"/>
-      <c r="U3" s="128"/>
-      <c r="V3" s="128"/>
-      <c r="W3" s="128"/>
-      <c r="X3" s="129"/>
-      <c r="Y3" s="129"/>
-      <c r="Z3" s="129"/>
-      <c r="AA3" s="129" t="s">
+      <c r="S3" s="152"/>
+      <c r="T3" s="152"/>
+      <c r="U3" s="152"/>
+      <c r="V3" s="152"/>
+      <c r="W3" s="152"/>
+      <c r="X3" s="106"/>
+      <c r="Y3" s="106"/>
+      <c r="Z3" s="106"/>
+      <c r="AA3" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="129"/>
-      <c r="AC3" s="129"/>
-      <c r="AD3" s="129" t="s">
+      <c r="AB3" s="106"/>
+      <c r="AC3" s="106"/>
+      <c r="AD3" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="AE3" s="129"/>
-      <c r="AF3" s="129"/>
-      <c r="AG3" s="129" t="s">
+      <c r="AE3" s="106"/>
+      <c r="AF3" s="106"/>
+      <c r="AG3" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="AH3" s="129"/>
-      <c r="AI3" s="129"/>
-      <c r="AJ3" s="129" t="s">
+      <c r="AH3" s="106"/>
+      <c r="AI3" s="106"/>
+      <c r="AJ3" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="AK3" s="129"/>
-      <c r="AL3" s="128" t="s">
+      <c r="AK3" s="106"/>
+      <c r="AL3" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="AM3" s="128"/>
-      <c r="AN3" s="127"/>
-    </row>
-    <row r="4" spans="1:40" s="125" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="127"/>
-      <c r="B4" s="131" t="s">
+      <c r="AM3" s="152"/>
+      <c r="AN3" s="105"/>
+    </row>
+    <row r="4" spans="1:40" s="103" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="105"/>
+      <c r="B4" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="132" t="s">
+      <c r="C4" s="153"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="132" t="s">
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="132" t="s">
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="N4" s="132" t="s">
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="130"/>
-      <c r="P4" s="130"/>
-      <c r="Q4" s="130"/>
-      <c r="R4" s="131" t="s">
+      <c r="O4" s="107"/>
+      <c r="P4" s="107"/>
+      <c r="Q4" s="107"/>
+      <c r="R4" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="131"/>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="131"/>
-      <c r="W4" s="131"/>
-      <c r="X4" s="129"/>
-      <c r="Y4" s="129"/>
-      <c r="Z4" s="129"/>
-      <c r="AA4" s="132" t="s">
+      <c r="S4" s="153"/>
+      <c r="T4" s="153"/>
+      <c r="U4" s="153"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="106"/>
+      <c r="Y4" s="106"/>
+      <c r="Z4" s="106"/>
+      <c r="AA4" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="AB4" s="129"/>
-      <c r="AC4" s="129"/>
-      <c r="AD4" s="132" t="s">
+      <c r="AB4" s="106"/>
+      <c r="AC4" s="106"/>
+      <c r="AD4" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="AE4" s="129"/>
-      <c r="AF4" s="129"/>
-      <c r="AG4" s="132" t="s">
+      <c r="AE4" s="106"/>
+      <c r="AF4" s="106"/>
+      <c r="AG4" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="AH4" s="129"/>
-      <c r="AI4" s="129"/>
-      <c r="AJ4" s="132" t="s">
+      <c r="AH4" s="106"/>
+      <c r="AI4" s="106"/>
+      <c r="AJ4" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="AK4" s="129"/>
-      <c r="AL4" s="131" t="s">
+      <c r="AK4" s="106"/>
+      <c r="AL4" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="AM4" s="131"/>
-      <c r="AN4" s="127"/>
-    </row>
-    <row r="5" spans="1:40" s="126" customFormat="1" ht="6.75" customHeight="1">
-      <c r="A5" s="133"/>
-      <c r="B5" s="134"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="137"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="137"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="137"/>
-      <c r="O5" s="138"/>
-      <c r="P5" s="139"/>
-      <c r="Q5" s="139"/>
-      <c r="R5" s="136"/>
-      <c r="S5" s="136"/>
-      <c r="T5" s="136"/>
-      <c r="U5" s="136"/>
-      <c r="V5" s="136"/>
-      <c r="W5" s="136"/>
-      <c r="X5" s="136"/>
-      <c r="Y5" s="136"/>
-      <c r="Z5" s="137"/>
-      <c r="AA5" s="137"/>
-      <c r="AB5" s="136"/>
-      <c r="AC5" s="136"/>
-      <c r="AD5" s="137"/>
-      <c r="AE5" s="136"/>
-      <c r="AF5" s="136"/>
-      <c r="AG5" s="137"/>
-      <c r="AH5" s="136"/>
-      <c r="AI5" s="136"/>
-      <c r="AJ5" s="137"/>
-      <c r="AK5" s="136"/>
-      <c r="AL5" s="135"/>
-      <c r="AM5" s="134"/>
-      <c r="AN5" s="133"/>
+      <c r="AM4" s="153"/>
+      <c r="AN4" s="105"/>
+    </row>
+    <row r="5" spans="1:40" s="104" customFormat="1" ht="6.75" customHeight="1">
+      <c r="A5" s="109"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="113"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="115"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="112"/>
+      <c r="X5" s="112"/>
+      <c r="Y5" s="112"/>
+      <c r="Z5" s="113"/>
+      <c r="AA5" s="113"/>
+      <c r="AB5" s="112"/>
+      <c r="AC5" s="112"/>
+      <c r="AD5" s="113"/>
+      <c r="AE5" s="112"/>
+      <c r="AF5" s="112"/>
+      <c r="AG5" s="113"/>
+      <c r="AH5" s="112"/>
+      <c r="AI5" s="112"/>
+      <c r="AJ5" s="113"/>
+      <c r="AK5" s="112"/>
+      <c r="AL5" s="111"/>
+      <c r="AM5" s="110"/>
+      <c r="AN5" s="109"/>
     </row>
     <row r="6" spans="1:40" s="16" customFormat="1" ht="50" customHeight="1">
       <c r="A6" s="13"/>
@@ -2469,7 +2469,7 @@
       <c r="H22" s="66"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
-      <c r="K22" s="104"/>
+      <c r="K22" s="128"/>
       <c r="L22" s="39"/>
       <c r="M22" s="17"/>
       <c r="N22" s="84" t="s">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="AB22" s="20"/>
       <c r="AC22" s="29"/>
-      <c r="AD22" s="104"/>
+      <c r="AD22" s="128"/>
       <c r="AE22" s="20"/>
       <c r="AF22" s="20"/>
       <c r="AG22" s="82"/>
@@ -2519,7 +2519,7 @@
       <c r="H23" s="66"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
-      <c r="K23" s="104"/>
+      <c r="K23" s="128"/>
       <c r="L23" s="39"/>
       <c r="M23" s="23"/>
       <c r="N23" s="85"/>
@@ -2538,7 +2538,7 @@
       <c r="AA23" s="92"/>
       <c r="AB23" s="26"/>
       <c r="AC23" s="29"/>
-      <c r="AD23" s="104"/>
+      <c r="AD23" s="128"/>
       <c r="AE23" s="20"/>
       <c r="AF23" s="20"/>
       <c r="AG23" s="82"/>
@@ -3328,22 +3328,22 @@
       <c r="L39" s="17"/>
       <c r="M39" s="17"/>
       <c r="N39" s="79"/>
-      <c r="O39" s="114" t="s">
+      <c r="O39" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="P39" s="115"/>
-      <c r="Q39" s="116"/>
-      <c r="R39" s="117"/>
+      <c r="P39" s="141"/>
+      <c r="Q39" s="142"/>
+      <c r="R39" s="143"/>
       <c r="S39" s="47"/>
       <c r="T39" s="47"/>
       <c r="U39" s="47"/>
       <c r="V39" s="49"/>
-      <c r="W39" s="114" t="s">
+      <c r="W39" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="X39" s="116"/>
-      <c r="Y39" s="115"/>
-      <c r="Z39" s="117"/>
+      <c r="X39" s="142"/>
+      <c r="Y39" s="141"/>
+      <c r="Z39" s="143"/>
       <c r="AA39" s="82"/>
       <c r="AB39" s="20"/>
       <c r="AC39" s="20"/>
@@ -3374,18 +3374,18 @@
       <c r="L40" s="17"/>
       <c r="M40" s="17"/>
       <c r="N40" s="79"/>
-      <c r="O40" s="118"/>
-      <c r="P40" s="115"/>
-      <c r="Q40" s="119"/>
-      <c r="R40" s="120"/>
+      <c r="O40" s="144"/>
+      <c r="P40" s="141"/>
+      <c r="Q40" s="145"/>
+      <c r="R40" s="146"/>
       <c r="S40" s="47"/>
       <c r="T40" s="47"/>
       <c r="U40" s="47"/>
       <c r="V40" s="49"/>
-      <c r="W40" s="118"/>
-      <c r="X40" s="119"/>
-      <c r="Y40" s="115"/>
-      <c r="Z40" s="120"/>
+      <c r="W40" s="144"/>
+      <c r="X40" s="145"/>
+      <c r="Y40" s="141"/>
+      <c r="Z40" s="146"/>
       <c r="AA40" s="82"/>
       <c r="AB40" s="20"/>
       <c r="AC40" s="20"/>
@@ -3567,14 +3567,14 @@
       <c r="O44" s="79"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="17"/>
-      <c r="R44" s="108" t="s">
+      <c r="R44" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="S44" s="109"/>
-      <c r="T44" s="109"/>
-      <c r="U44" s="109"/>
-      <c r="V44" s="109"/>
-      <c r="W44" s="110"/>
+      <c r="S44" s="133"/>
+      <c r="T44" s="133"/>
+      <c r="U44" s="133"/>
+      <c r="V44" s="133"/>
+      <c r="W44" s="134"/>
       <c r="X44" s="20"/>
       <c r="Y44" s="29"/>
       <c r="Z44" s="82"/>
@@ -3617,12 +3617,12 @@
       <c r="O45" s="79"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="17"/>
-      <c r="R45" s="111"/>
-      <c r="S45" s="112"/>
-      <c r="T45" s="112"/>
-      <c r="U45" s="112"/>
-      <c r="V45" s="112"/>
-      <c r="W45" s="113"/>
+      <c r="R45" s="135"/>
+      <c r="S45" s="136"/>
+      <c r="T45" s="136"/>
+      <c r="U45" s="136"/>
+      <c r="V45" s="136"/>
+      <c r="W45" s="137"/>
       <c r="X45" s="20"/>
       <c r="Y45" s="29"/>
       <c r="Z45" s="82"/>
@@ -3668,14 +3668,14 @@
       <c r="O46" s="79"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="17"/>
-      <c r="R46" s="123" t="s">
+      <c r="R46" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="S46" s="123"/>
-      <c r="T46" s="123"/>
-      <c r="U46" s="123"/>
-      <c r="V46" s="123"/>
-      <c r="W46" s="123"/>
+      <c r="S46" s="149"/>
+      <c r="T46" s="149"/>
+      <c r="U46" s="149"/>
+      <c r="V46" s="149"/>
+      <c r="W46" s="149"/>
       <c r="X46" s="20"/>
       <c r="Y46" s="29"/>
       <c r="Z46" s="82"/>
@@ -3723,12 +3723,12 @@
       <c r="O47" s="79"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="17"/>
-      <c r="R47" s="124"/>
-      <c r="S47" s="124"/>
-      <c r="T47" s="124"/>
-      <c r="U47" s="124"/>
-      <c r="V47" s="124"/>
-      <c r="W47" s="124"/>
+      <c r="R47" s="150"/>
+      <c r="S47" s="150"/>
+      <c r="T47" s="150"/>
+      <c r="U47" s="150"/>
+      <c r="V47" s="150"/>
+      <c r="W47" s="150"/>
       <c r="X47" s="20"/>
       <c r="Y47" s="29"/>
       <c r="Z47" s="82"/>
@@ -3870,10 +3870,10 @@
       <c r="P50" s="39"/>
       <c r="Q50" s="17"/>
       <c r="R50" s="17"/>
-      <c r="S50" s="122"/>
-      <c r="T50" s="122"/>
-      <c r="U50" s="122"/>
-      <c r="V50" s="122"/>
+      <c r="S50" s="148"/>
+      <c r="T50" s="148"/>
+      <c r="U50" s="148"/>
+      <c r="V50" s="148"/>
       <c r="W50" s="20"/>
       <c r="X50" s="20"/>
       <c r="Y50" s="29"/>
@@ -3920,10 +3920,10 @@
       <c r="P51" s="39"/>
       <c r="Q51" s="17"/>
       <c r="R51" s="17"/>
-      <c r="S51" s="121"/>
-      <c r="T51" s="121"/>
-      <c r="U51" s="121"/>
-      <c r="V51" s="121"/>
+      <c r="S51" s="147"/>
+      <c r="T51" s="147"/>
+      <c r="U51" s="147"/>
+      <c r="V51" s="147"/>
       <c r="W51" s="20"/>
       <c r="X51" s="20"/>
       <c r="Y51" s="29"/>
@@ -3972,10 +3972,10 @@
       <c r="P52" s="39"/>
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
-      <c r="S52" s="121"/>
-      <c r="T52" s="121"/>
-      <c r="U52" s="121"/>
-      <c r="V52" s="121"/>
+      <c r="S52" s="147"/>
+      <c r="T52" s="147"/>
+      <c r="U52" s="147"/>
+      <c r="V52" s="147"/>
       <c r="W52" s="20"/>
       <c r="X52" s="20"/>
       <c r="Y52" s="29"/>
@@ -4022,10 +4022,10 @@
       <c r="P53" s="39"/>
       <c r="Q53" s="17"/>
       <c r="R53" s="17"/>
-      <c r="S53" s="121"/>
-      <c r="T53" s="121"/>
-      <c r="U53" s="121"/>
-      <c r="V53" s="121"/>
+      <c r="S53" s="147"/>
+      <c r="T53" s="147"/>
+      <c r="U53" s="147"/>
+      <c r="V53" s="147"/>
       <c r="W53" s="20"/>
       <c r="X53" s="20"/>
       <c r="Y53" s="29"/>
@@ -4075,12 +4075,12 @@
       <c r="O54" s="79"/>
       <c r="P54" s="39"/>
       <c r="Q54" s="17"/>
-      <c r="R54" s="122"/>
-      <c r="S54" s="122"/>
-      <c r="T54" s="122"/>
-      <c r="U54" s="122"/>
-      <c r="V54" s="122"/>
-      <c r="W54" s="122"/>
+      <c r="R54" s="148"/>
+      <c r="S54" s="148"/>
+      <c r="T54" s="148"/>
+      <c r="U54" s="148"/>
+      <c r="V54" s="148"/>
+      <c r="W54" s="148"/>
       <c r="X54" s="20"/>
       <c r="Y54" s="29"/>
       <c r="Z54" s="82"/>
@@ -4132,12 +4132,12 @@
       <c r="O55" s="79"/>
       <c r="P55" s="39"/>
       <c r="Q55" s="17"/>
-      <c r="R55" s="122"/>
-      <c r="S55" s="122"/>
-      <c r="T55" s="122"/>
-      <c r="U55" s="122"/>
-      <c r="V55" s="122"/>
-      <c r="W55" s="122"/>
+      <c r="R55" s="148"/>
+      <c r="S55" s="148"/>
+      <c r="T55" s="148"/>
+      <c r="U55" s="148"/>
+      <c r="V55" s="148"/>
+      <c r="W55" s="148"/>
       <c r="X55" s="20"/>
       <c r="Y55" s="29"/>
       <c r="Z55" s="82"/>
@@ -4228,7 +4228,7 @@
       <c r="H57" s="66"/>
       <c r="I57" s="19"/>
       <c r="J57" s="19"/>
-      <c r="K57" s="104"/>
+      <c r="K57" s="128"/>
       <c r="L57" s="39"/>
       <c r="M57" s="31"/>
       <c r="N57" s="84" t="s">
@@ -4251,8 +4251,8 @@
       </c>
       <c r="AB57" s="35"/>
       <c r="AC57" s="29"/>
-      <c r="AD57" s="105"/>
-      <c r="AE57" s="106"/>
+      <c r="AD57" s="129"/>
+      <c r="AE57" s="130"/>
       <c r="AF57" s="20"/>
       <c r="AG57" s="82"/>
       <c r="AH57" s="20"/>
@@ -4278,7 +4278,7 @@
       <c r="H58" s="66"/>
       <c r="I58" s="19"/>
       <c r="J58" s="19"/>
-      <c r="K58" s="104"/>
+      <c r="K58" s="128"/>
       <c r="L58" s="39"/>
       <c r="M58" s="17"/>
       <c r="N58" s="82"/>
@@ -4297,8 +4297,8 @@
       <c r="AA58" s="82"/>
       <c r="AB58" s="20"/>
       <c r="AC58" s="29"/>
-      <c r="AD58" s="106"/>
-      <c r="AE58" s="106"/>
+      <c r="AD58" s="130"/>
+      <c r="AE58" s="130"/>
       <c r="AF58" s="20"/>
       <c r="AG58" s="82"/>
       <c r="AH58" s="20"/>
@@ -4333,18 +4333,18 @@
       <c r="L59" s="39"/>
       <c r="M59" s="17"/>
       <c r="N59" s="79"/>
-      <c r="O59" s="141"/>
-      <c r="P59" s="142"/>
-      <c r="Q59" s="142"/>
-      <c r="R59" s="143"/>
-      <c r="S59" s="143"/>
-      <c r="T59" s="143"/>
-      <c r="U59" s="143"/>
-      <c r="V59" s="143"/>
-      <c r="W59" s="143"/>
-      <c r="X59" s="144"/>
-      <c r="Y59" s="144"/>
-      <c r="Z59" s="145"/>
+      <c r="O59" s="116"/>
+      <c r="P59" s="117"/>
+      <c r="Q59" s="117"/>
+      <c r="R59" s="151"/>
+      <c r="S59" s="151"/>
+      <c r="T59" s="151"/>
+      <c r="U59" s="151"/>
+      <c r="V59" s="151"/>
+      <c r="W59" s="151"/>
+      <c r="X59" s="118"/>
+      <c r="Y59" s="118"/>
+      <c r="Z59" s="119"/>
       <c r="AA59" s="82"/>
       <c r="AB59" s="20"/>
       <c r="AC59" s="29"/>
@@ -4384,18 +4384,18 @@
       <c r="L60" s="39"/>
       <c r="M60" s="17"/>
       <c r="N60" s="79"/>
-      <c r="O60" s="141"/>
-      <c r="P60" s="142"/>
-      <c r="Q60" s="142"/>
-      <c r="R60" s="142"/>
-      <c r="S60" s="146"/>
-      <c r="T60" s="146"/>
-      <c r="U60" s="146"/>
-      <c r="V60" s="144"/>
-      <c r="W60" s="144"/>
-      <c r="X60" s="144"/>
-      <c r="Y60" s="144"/>
-      <c r="Z60" s="145"/>
+      <c r="O60" s="116"/>
+      <c r="P60" s="117"/>
+      <c r="Q60" s="117"/>
+      <c r="R60" s="117"/>
+      <c r="S60" s="120"/>
+      <c r="T60" s="120"/>
+      <c r="U60" s="120"/>
+      <c r="V60" s="118"/>
+      <c r="W60" s="118"/>
+      <c r="X60" s="118"/>
+      <c r="Y60" s="118"/>
+      <c r="Z60" s="119"/>
       <c r="AA60" s="82"/>
       <c r="AB60" s="20"/>
       <c r="AC60" s="29"/>
@@ -4432,18 +4432,18 @@
       <c r="L61" s="39"/>
       <c r="M61" s="17"/>
       <c r="N61" s="79"/>
-      <c r="O61" s="141"/>
-      <c r="P61" s="142"/>
-      <c r="Q61" s="142"/>
-      <c r="R61" s="142"/>
-      <c r="S61" s="146"/>
-      <c r="T61" s="146"/>
-      <c r="U61" s="146"/>
-      <c r="V61" s="144"/>
-      <c r="W61" s="144"/>
-      <c r="X61" s="144"/>
-      <c r="Y61" s="144"/>
-      <c r="Z61" s="145"/>
+      <c r="O61" s="116"/>
+      <c r="P61" s="117"/>
+      <c r="Q61" s="117"/>
+      <c r="R61" s="117"/>
+      <c r="S61" s="120"/>
+      <c r="T61" s="120"/>
+      <c r="U61" s="120"/>
+      <c r="V61" s="118"/>
+      <c r="W61" s="118"/>
+      <c r="X61" s="118"/>
+      <c r="Y61" s="118"/>
+      <c r="Z61" s="119"/>
       <c r="AA61" s="82"/>
       <c r="AB61" s="20"/>
       <c r="AC61" s="29"/>
@@ -4483,18 +4483,18 @@
       <c r="L62" s="39"/>
       <c r="M62" s="17"/>
       <c r="N62" s="79"/>
-      <c r="O62" s="147"/>
-      <c r="P62" s="148"/>
-      <c r="Q62" s="148"/>
-      <c r="R62" s="148"/>
-      <c r="S62" s="149"/>
-      <c r="T62" s="150"/>
-      <c r="U62" s="146"/>
-      <c r="V62" s="151"/>
-      <c r="W62" s="152"/>
-      <c r="X62" s="152"/>
-      <c r="Y62" s="152"/>
-      <c r="Z62" s="152"/>
+      <c r="O62" s="121"/>
+      <c r="P62" s="122"/>
+      <c r="Q62" s="122"/>
+      <c r="R62" s="122"/>
+      <c r="S62" s="123"/>
+      <c r="T62" s="124"/>
+      <c r="U62" s="120"/>
+      <c r="V62" s="125"/>
+      <c r="W62" s="139"/>
+      <c r="X62" s="139"/>
+      <c r="Y62" s="139"/>
+      <c r="Z62" s="139"/>
       <c r="AA62" s="82"/>
       <c r="AB62" s="20"/>
       <c r="AC62" s="29"/>
@@ -4536,18 +4536,18 @@
       <c r="L63" s="39"/>
       <c r="M63" s="17"/>
       <c r="N63" s="79"/>
-      <c r="O63" s="153"/>
-      <c r="P63" s="154"/>
-      <c r="Q63" s="154"/>
-      <c r="R63" s="154"/>
-      <c r="S63" s="154"/>
-      <c r="T63" s="150"/>
-      <c r="U63" s="146"/>
-      <c r="V63" s="153"/>
-      <c r="W63" s="153"/>
-      <c r="X63" s="153"/>
-      <c r="Y63" s="153"/>
-      <c r="Z63" s="153"/>
+      <c r="O63" s="126"/>
+      <c r="P63" s="127"/>
+      <c r="Q63" s="127"/>
+      <c r="R63" s="127"/>
+      <c r="S63" s="127"/>
+      <c r="T63" s="124"/>
+      <c r="U63" s="120"/>
+      <c r="V63" s="126"/>
+      <c r="W63" s="126"/>
+      <c r="X63" s="126"/>
+      <c r="Y63" s="126"/>
+      <c r="Z63" s="126"/>
       <c r="AA63" s="82"/>
       <c r="AB63" s="20"/>
       <c r="AC63" s="29"/>
@@ -4588,18 +4588,18 @@
       <c r="L64" s="38"/>
       <c r="M64" s="17"/>
       <c r="N64" s="79"/>
-      <c r="O64" s="147"/>
-      <c r="P64" s="148"/>
-      <c r="Q64" s="148"/>
-      <c r="R64" s="148"/>
-      <c r="S64" s="149"/>
-      <c r="T64" s="150"/>
-      <c r="U64" s="146"/>
-      <c r="V64" s="151"/>
-      <c r="W64" s="152"/>
-      <c r="X64" s="152"/>
-      <c r="Y64" s="152"/>
-      <c r="Z64" s="152"/>
+      <c r="O64" s="121"/>
+      <c r="P64" s="122"/>
+      <c r="Q64" s="122"/>
+      <c r="R64" s="122"/>
+      <c r="S64" s="123"/>
+      <c r="T64" s="124"/>
+      <c r="U64" s="120"/>
+      <c r="V64" s="125"/>
+      <c r="W64" s="139"/>
+      <c r="X64" s="139"/>
+      <c r="Y64" s="139"/>
+      <c r="Z64" s="139"/>
       <c r="AA64" s="82"/>
       <c r="AB64" s="20"/>
       <c r="AC64" s="29"/>
@@ -4638,18 +4638,18 @@
       <c r="L65" s="45"/>
       <c r="M65" s="17"/>
       <c r="N65" s="79"/>
-      <c r="O65" s="155"/>
-      <c r="P65" s="155"/>
-      <c r="Q65" s="155"/>
-      <c r="R65" s="155"/>
-      <c r="S65" s="155"/>
-      <c r="T65" s="146"/>
-      <c r="U65" s="146"/>
-      <c r="V65" s="156"/>
-      <c r="W65" s="156"/>
-      <c r="X65" s="156"/>
-      <c r="Y65" s="156"/>
-      <c r="Z65" s="156"/>
+      <c r="O65" s="156"/>
+      <c r="P65" s="156"/>
+      <c r="Q65" s="156"/>
+      <c r="R65" s="156"/>
+      <c r="S65" s="156"/>
+      <c r="T65" s="120"/>
+      <c r="U65" s="120"/>
+      <c r="V65" s="157"/>
+      <c r="W65" s="157"/>
+      <c r="X65" s="157"/>
+      <c r="Y65" s="157"/>
+      <c r="Z65" s="157"/>
       <c r="AA65" s="82"/>
       <c r="AB65" s="20"/>
       <c r="AC65" s="34"/>
@@ -4686,18 +4686,18 @@
       <c r="L66" s="20"/>
       <c r="M66" s="17"/>
       <c r="N66" s="79"/>
-      <c r="O66" s="153"/>
-      <c r="P66" s="154"/>
-      <c r="Q66" s="154"/>
-      <c r="R66" s="154"/>
-      <c r="S66" s="154"/>
-      <c r="T66" s="146"/>
-      <c r="U66" s="146"/>
-      <c r="V66" s="145"/>
-      <c r="W66" s="145"/>
-      <c r="X66" s="145"/>
-      <c r="Y66" s="145"/>
-      <c r="Z66" s="145"/>
+      <c r="O66" s="126"/>
+      <c r="P66" s="127"/>
+      <c r="Q66" s="127"/>
+      <c r="R66" s="127"/>
+      <c r="S66" s="127"/>
+      <c r="T66" s="120"/>
+      <c r="U66" s="120"/>
+      <c r="V66" s="119"/>
+      <c r="W66" s="119"/>
+      <c r="X66" s="119"/>
+      <c r="Y66" s="119"/>
+      <c r="Z66" s="119"/>
       <c r="AA66" s="82"/>
       <c r="AB66" s="20"/>
       <c r="AC66" s="20"/>
@@ -4737,18 +4737,18 @@
       <c r="L67" s="17"/>
       <c r="M67" s="17"/>
       <c r="N67" s="79"/>
-      <c r="O67" s="147"/>
-      <c r="P67" s="148"/>
-      <c r="Q67" s="148"/>
-      <c r="R67" s="148"/>
-      <c r="S67" s="149"/>
-      <c r="T67" s="146"/>
-      <c r="U67" s="146"/>
-      <c r="V67" s="151"/>
-      <c r="W67" s="152"/>
-      <c r="X67" s="152"/>
-      <c r="Y67" s="152"/>
-      <c r="Z67" s="152"/>
+      <c r="O67" s="121"/>
+      <c r="P67" s="122"/>
+      <c r="Q67" s="122"/>
+      <c r="R67" s="122"/>
+      <c r="S67" s="123"/>
+      <c r="T67" s="120"/>
+      <c r="U67" s="120"/>
+      <c r="V67" s="125"/>
+      <c r="W67" s="139"/>
+      <c r="X67" s="139"/>
+      <c r="Y67" s="139"/>
+      <c r="Z67" s="139"/>
       <c r="AA67" s="82"/>
       <c r="AB67" s="20"/>
       <c r="AC67" s="20"/>
@@ -4790,18 +4790,18 @@
       <c r="L68" s="17"/>
       <c r="M68" s="17"/>
       <c r="N68" s="79"/>
-      <c r="O68" s="153"/>
-      <c r="P68" s="154"/>
-      <c r="Q68" s="154"/>
-      <c r="R68" s="154"/>
-      <c r="S68" s="154"/>
-      <c r="T68" s="150"/>
-      <c r="U68" s="146"/>
-      <c r="V68" s="153"/>
-      <c r="W68" s="153"/>
-      <c r="X68" s="153"/>
-      <c r="Y68" s="153"/>
-      <c r="Z68" s="153"/>
+      <c r="O68" s="126"/>
+      <c r="P68" s="127"/>
+      <c r="Q68" s="127"/>
+      <c r="R68" s="127"/>
+      <c r="S68" s="127"/>
+      <c r="T68" s="124"/>
+      <c r="U68" s="120"/>
+      <c r="V68" s="126"/>
+      <c r="W68" s="126"/>
+      <c r="X68" s="126"/>
+      <c r="Y68" s="126"/>
+      <c r="Z68" s="126"/>
       <c r="AA68" s="82"/>
       <c r="AB68" s="20"/>
       <c r="AC68" s="20"/>
@@ -4840,18 +4840,18 @@
       <c r="L69" s="17"/>
       <c r="M69" s="17"/>
       <c r="N69" s="79"/>
-      <c r="O69" s="157"/>
-      <c r="P69" s="157"/>
-      <c r="Q69" s="157"/>
-      <c r="R69" s="157"/>
-      <c r="S69" s="149"/>
-      <c r="T69" s="150"/>
-      <c r="U69" s="146"/>
-      <c r="V69" s="151"/>
-      <c r="W69" s="152"/>
-      <c r="X69" s="152"/>
-      <c r="Y69" s="152"/>
-      <c r="Z69" s="152"/>
+      <c r="O69" s="138"/>
+      <c r="P69" s="138"/>
+      <c r="Q69" s="138"/>
+      <c r="R69" s="138"/>
+      <c r="S69" s="123"/>
+      <c r="T69" s="124"/>
+      <c r="U69" s="120"/>
+      <c r="V69" s="125"/>
+      <c r="W69" s="139"/>
+      <c r="X69" s="139"/>
+      <c r="Y69" s="139"/>
+      <c r="Z69" s="139"/>
       <c r="AA69" s="82"/>
       <c r="AB69" s="20"/>
       <c r="AC69" s="20"/>
@@ -4891,18 +4891,18 @@
       <c r="L70" s="17"/>
       <c r="M70" s="17"/>
       <c r="N70" s="79"/>
-      <c r="O70" s="140"/>
-      <c r="P70" s="140"/>
-      <c r="Q70" s="140"/>
-      <c r="R70" s="140"/>
-      <c r="S70" s="140"/>
+      <c r="O70" s="155"/>
+      <c r="P70" s="155"/>
+      <c r="Q70" s="155"/>
+      <c r="R70" s="155"/>
+      <c r="S70" s="155"/>
       <c r="T70" s="13"/>
       <c r="U70" s="13"/>
-      <c r="V70" s="140"/>
-      <c r="W70" s="140"/>
-      <c r="X70" s="140"/>
-      <c r="Y70" s="140"/>
-      <c r="Z70" s="140"/>
+      <c r="V70" s="155"/>
+      <c r="W70" s="155"/>
+      <c r="X70" s="155"/>
+      <c r="Y70" s="155"/>
+      <c r="Z70" s="155"/>
       <c r="AA70" s="82"/>
       <c r="AB70" s="20"/>
       <c r="AC70" s="20"/>
@@ -4986,20 +4986,20 @@
       <c r="L72" s="17"/>
       <c r="M72" s="17"/>
       <c r="N72" s="66"/>
-      <c r="O72" s="103" t="s">
+      <c r="O72" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="P72" s="103"/>
-      <c r="Q72" s="103"/>
-      <c r="R72" s="103"/>
-      <c r="S72" s="103"/>
-      <c r="T72" s="103"/>
-      <c r="U72" s="103"/>
-      <c r="V72" s="103"/>
-      <c r="W72" s="103"/>
-      <c r="X72" s="103"/>
-      <c r="Y72" s="103"/>
-      <c r="Z72" s="103"/>
+      <c r="P72" s="154"/>
+      <c r="Q72" s="154"/>
+      <c r="R72" s="154"/>
+      <c r="S72" s="154"/>
+      <c r="T72" s="154"/>
+      <c r="U72" s="154"/>
+      <c r="V72" s="154"/>
+      <c r="W72" s="154"/>
+      <c r="X72" s="154"/>
+      <c r="Y72" s="154"/>
+      <c r="Z72" s="154"/>
       <c r="AA72" s="82"/>
       <c r="AB72" s="20"/>
       <c r="AC72" s="20"/>
@@ -5034,18 +5034,18 @@
       <c r="L73" s="13"/>
       <c r="M73" s="13"/>
       <c r="N73" s="88"/>
-      <c r="O73" s="103"/>
-      <c r="P73" s="103"/>
-      <c r="Q73" s="103"/>
-      <c r="R73" s="103"/>
-      <c r="S73" s="103"/>
-      <c r="T73" s="103"/>
-      <c r="U73" s="103"/>
-      <c r="V73" s="103"/>
-      <c r="W73" s="103"/>
-      <c r="X73" s="103"/>
-      <c r="Y73" s="103"/>
-      <c r="Z73" s="103"/>
+      <c r="O73" s="154"/>
+      <c r="P73" s="154"/>
+      <c r="Q73" s="154"/>
+      <c r="R73" s="154"/>
+      <c r="S73" s="154"/>
+      <c r="T73" s="154"/>
+      <c r="U73" s="154"/>
+      <c r="V73" s="154"/>
+      <c r="W73" s="154"/>
+      <c r="X73" s="154"/>
+      <c r="Y73" s="154"/>
+      <c r="Z73" s="154"/>
       <c r="AA73" s="89"/>
       <c r="AB73" s="13"/>
       <c r="AC73" s="13"/>
@@ -5076,18 +5076,18 @@
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
       <c r="N74" s="89"/>
-      <c r="O74" s="103"/>
-      <c r="P74" s="103"/>
-      <c r="Q74" s="103"/>
-      <c r="R74" s="103"/>
-      <c r="S74" s="103"/>
-      <c r="T74" s="103"/>
-      <c r="U74" s="103"/>
-      <c r="V74" s="103"/>
-      <c r="W74" s="103"/>
-      <c r="X74" s="103"/>
-      <c r="Y74" s="103"/>
-      <c r="Z74" s="103"/>
+      <c r="O74" s="154"/>
+      <c r="P74" s="154"/>
+      <c r="Q74" s="154"/>
+      <c r="R74" s="154"/>
+      <c r="S74" s="154"/>
+      <c r="T74" s="154"/>
+      <c r="U74" s="154"/>
+      <c r="V74" s="154"/>
+      <c r="W74" s="154"/>
+      <c r="X74" s="154"/>
+      <c r="Y74" s="154"/>
+      <c r="Z74" s="154"/>
       <c r="AA74" s="89"/>
       <c r="AB74" s="8"/>
       <c r="AC74" s="8"/>
@@ -5246,6 +5246,19 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="29">
+    <mergeCell ref="O72:Z74"/>
+    <mergeCell ref="V70:Z70"/>
+    <mergeCell ref="O70:S70"/>
+    <mergeCell ref="O65:S65"/>
+    <mergeCell ref="V65:Z65"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="AD22:AD23"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="R3:W3"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="R4:W4"/>
     <mergeCell ref="K57:K58"/>
     <mergeCell ref="AD57:AE58"/>
     <mergeCell ref="A1:AN2"/>
@@ -5262,19 +5275,6 @@
     <mergeCell ref="W64:Z64"/>
     <mergeCell ref="R54:W55"/>
     <mergeCell ref="W62:Z62"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="AD22:AD23"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="R3:W3"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R4:W4"/>
-    <mergeCell ref="O72:Z74"/>
-    <mergeCell ref="V70:Z70"/>
-    <mergeCell ref="O70:S70"/>
-    <mergeCell ref="O65:S65"/>
-    <mergeCell ref="V65:Z65"/>
   </mergeCells>
   <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ8 AJ71 AJ67 AJ63 AJ59 AJ55 AJ51 AJ47 AJ43 AJ36 AJ32 AJ28 AJ24 AJ20 AJ16 AJ12">

</xml_diff>